<commit_message>
past days optimization on streamlit
</commit_message>
<xml_diff>
--- a/Data/transformed_data/categorised_articles.xlsx
+++ b/Data/transformed_data/categorised_articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work - Data\Projects\GitHub\BiscuitLab\how_many\Data\transformed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBE5BC3-820C-4AD1-A5DE-970363434DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAE5D8A-D952-4124-B7BD-3171674D48B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{361B175B-E084-4367-9EB1-3B87CE7960A5}"/>
   </bookViews>
@@ -4218,8 +4218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4849CFB-BDB6-4E4E-9A5A-306710772CA3}">
   <dimension ref="A1:E538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
+      <selection activeCell="A534" sqref="A534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12219,8 +12219,8 @@
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A533" s="3" t="s">
-        <v>2</v>
+      <c r="A533" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="B533" s="3" t="s">
         <v>325</v>
@@ -12234,8 +12234,8 @@
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A534" s="3" t="s">
-        <v>2</v>
+      <c r="A534" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="B534" s="3" t="s">
         <v>326</v>
@@ -12250,7 +12250,7 @@
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
-        <v>2</v>
+        <v>228</v>
       </c>
       <c r="B535" s="2" t="s">
         <v>225</v>
@@ -12264,8 +12264,8 @@
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A536" s="3" t="s">
-        <v>2</v>
+      <c r="A536" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="B536" s="3" t="s">
         <v>225</v>

</xml_diff>